<commit_message>
Implemented people shiny interface
Implemented tools for people metadata lists
</commit_message>
<xml_diff>
--- a/test/01_input/meta/people.xlsx
+++ b/test/01_input/meta/people.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e07181b91a604cdb/git_repo/metadata/test/01_input/meta/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v78h241\Box\UCFR LTREB 2017 - 2022\DataWorking\Metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{1121A4EB-DDFD-418B-8D0F-D0B3B17822E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F2DA88A-DE48-4102-AC5E-EE4231E39737}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2E761F-DC56-40EB-A1D8-389F5E23C96B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2970" yWindow="1290" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Funding" sheetId="2" r:id="rId2"/>
+    <sheet name="Funding" sheetId="3" r:id="rId2"/>
+    <sheet name="CRediT Taxonomy" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="135">
   <si>
     <t>givenName</t>
   </si>
@@ -281,31 +282,169 @@
     </r>
   </si>
   <si>
+    <t>Link:</t>
+  </si>
+  <si>
+    <t>https://casrai.org/credit/</t>
+  </si>
+  <si>
+    <t>Conceptualization</t>
+  </si>
+  <si>
+    <t>Data curation</t>
+  </si>
+  <si>
+    <t>Formal Analysis</t>
+  </si>
+  <si>
+    <t>Funding acquisition</t>
+  </si>
+  <si>
+    <t>Investigation</t>
+  </si>
+  <si>
+    <t>Methodology</t>
+  </si>
+  <si>
+    <t>Project administration</t>
+  </si>
+  <si>
+    <t>Resources</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>Supervision</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t>Visualization</t>
+  </si>
+  <si>
+    <t>Writing – original draft</t>
+  </si>
+  <si>
+    <t>Writing – review &amp; editing</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Management activities to annotate (produce metadata), scrub data and maintain research data (including software code, where it is necessary for interpreting the data itself) for initial use and later re-use.</t>
+  </si>
+  <si>
+    <t>Ideas; formulation or evolution of overarching research goals and aims.</t>
+  </si>
+  <si>
+    <t>Application of statistical, mathematical, computational, or other formal techniques to analyze or synthesize study data.</t>
+  </si>
+  <si>
+    <t>Acquisition of the financial support for the project leading to this publication.</t>
+  </si>
+  <si>
+    <t>Conducting a research and investigation process, specifically performing the experiments, or data/evidence collection.</t>
+  </si>
+  <si>
+    <t>Development or design of methodology; creation of models.</t>
+  </si>
+  <si>
+    <t>Management and coordination responsibility for the research activity planning and execution.</t>
+  </si>
+  <si>
+    <t>Provision of study materials, reagents, materials, patients, laboratory samples, animals, instrumentation, computing resources, or other analysis tools.</t>
+  </si>
+  <si>
+    <t>Programming, software development; designing computer programs; implementation of the computer code and supporting algorithms; testing of existing code components.</t>
+  </si>
+  <si>
+    <t>Oversight and leadership responsibility for the research activity planning and execution, including mentorship external to the core team.</t>
+  </si>
+  <si>
+    <t>Verification, whether as a part of the activity or separate, of the overall replication/reproducibility of results/experiments and other research outputs.</t>
+  </si>
+  <si>
+    <t>Preparation, creation and/or presentation of the published work, specifically visualization/data presentation.</t>
+  </si>
+  <si>
+    <t>Preparation, creation and/or presentation of the published work, specifically writing the initial draft (including substantive translation).</t>
+  </si>
+  <si>
+    <t>Preparation, creation and/or presentation of the published work by those from the original research group, specifically critical review, commentary or revision – including pre- or post-publication stages.</t>
+  </si>
+  <si>
+    <t>PatrickH</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>Hurley</t>
+  </si>
+  <si>
+    <t>patrick.hurley@umontana.edu</t>
+  </si>
+  <si>
+    <t>RoyceE</t>
+  </si>
+  <si>
+    <t>Royce</t>
+  </si>
+  <si>
+    <t>Engstrom</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>royce.engstrom@umontana.edu</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>TaylorGQ</t>
+  </si>
+  <si>
+    <t>Gold Quiros</t>
+  </si>
+  <si>
+    <t>taylor.goldquiros@umontana.edu</t>
+  </si>
+  <si>
+    <t>0000-0003-3721-6027</t>
+  </si>
+  <si>
+    <t>projectTitle</t>
+  </si>
+  <si>
+    <t>fundingAgency</t>
+  </si>
+  <si>
+    <t>fundingNumber</t>
+  </si>
+  <si>
+    <t>RobP_LTREB</t>
+  </si>
+  <si>
+    <t>LTREB: Collaborative research - River ecosystem responses to floodplain restoration</t>
+  </si>
+  <si>
+    <t>US National Science Foundation</t>
+  </si>
+  <si>
     <t>MauryV_LTREB</t>
   </si>
   <si>
-    <t>RobP_LTREB</t>
-  </si>
-  <si>
     <t>RayC_EPSCOR</t>
   </si>
   <si>
-    <t>projectTitle</t>
-  </si>
-  <si>
-    <t>fundingAgency</t>
-  </si>
-  <si>
-    <t>fundingNumber</t>
-  </si>
-  <si>
-    <t>LTREB: Collaborative research - River ecosystem responses to floodplain restoration</t>
-  </si>
-  <si>
     <t>RII Track-1 Consortium for Research on Environmental Water Systems</t>
-  </si>
-  <si>
-    <t>US National Science Foundation</t>
   </si>
   <si>
     <t>OIA-1757351</t>
@@ -457,7 +596,9 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -780,7 +921,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -823,26 +964,41 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -876,6 +1032,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1196,10 +1353,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H16"/>
+  <dimension ref="B2:H19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1242,25 +1399,22 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="H5" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -1288,91 +1442,89 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
       </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="H7" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" t="s">
-        <v>25</v>
+      <c r="B8" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="H9" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>53</v>
+        <v>115</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>116</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>118</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>117</v>
       </c>
       <c r="F10" t="s">
         <v>8</v>
       </c>
       <c r="G10" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" t="s">
-        <v>35</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -1397,121 +1549,187 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>56</v>
+        <v>111</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>112</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="F12" t="s">
         <v>8</v>
       </c>
       <c r="G12" t="s">
-        <v>59</v>
-      </c>
-      <c r="H12" t="s">
-        <v>60</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>54</v>
+        <v>121</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>120</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>122</v>
       </c>
       <c r="F13" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="G13" t="s">
-        <v>39</v>
+        <v>123</v>
       </c>
       <c r="H13" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="E14" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="F14" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="G14" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="H14" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="F15" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="G15" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="H15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>44</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:H19">
+    <sortCondition ref="E5:E19"/>
+    <sortCondition ref="C5:C19"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D6DDA16-46D8-428B-B270-8CF9A9A3B1BF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C942C07-C81C-4449-98EF-60CBF6AC8708}">
   <dimension ref="B2:K7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
@@ -1556,113 +1774,260 @@
         <v>46</v>
       </c>
       <c r="I4" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="K5" s="11">
+        <v>1655198</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="K6" s="11">
+        <v>1655197</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" s="10" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6BBC608-0972-4F6B-8D57-175B779690F4}">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="26.85546875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="54.42578125" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E2" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="E3" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="F3" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E4" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="F4" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E5" s="7" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="4" t="s">
+      <c r="F5" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E6" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="F6" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E7" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E8" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="K5" s="6">
-        <v>1655198</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="K6" s="6">
-        <v>1655197</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="K7" s="7" t="s">
+      <c r="F8" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E9" s="7" t="s">
         <v>88</v>
       </c>
+      <c r="F9" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="E10" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E11" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E12" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E13" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E14" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="E15" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>110</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="19" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{1E7E320D-F786-4DEF-9374-580C9CEE72ED}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>